<commit_message>
Primer commit: Inicializando el proyecto
</commit_message>
<xml_diff>
--- a/Datos_DDRE.xlsx
+++ b/Datos_DDRE.xlsx
@@ -371,11 +371,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>